<commit_message>
RFID Wallet Antitheft/Scanning Leather Wallet Sale Price 1.399
</commit_message>
<xml_diff>
--- a/Inventory/inventory.tracker.xlsx
+++ b/Inventory/inventory.tracker.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -40,13 +40,19 @@
   </si>
   <si>
     <t>0001</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>RFID Wallet Antitheft/Scanning Leather wallet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +60,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,13 +91,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,7 +387,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -358,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -373,19 +410,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -403,6 +440,23 @@
         <v>1499</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>900</v>
+      </c>
+      <c r="D3">
+        <v>1.399</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flint Match Lighter Metal Outdoor Camping sale price 149.00
</commit_message>
<xml_diff>
--- a/Inventory/inventory.tracker.xlsx
+++ b/Inventory/inventory.tracker.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>RFID Wallet Antitheft/Scanning Leather wallet</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>Fling Match Lighter Metal Outdoor Camping</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -460,6 +466,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>149</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changed fling to flint
</commit_message>
<xml_diff>
--- a/Inventory/inventory.tracker.xlsx
+++ b/Inventory/inventory.tracker.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12645"/>
   </bookViews>
@@ -10,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -51,14 +51,14 @@
     <t>0003</t>
   </si>
   <si>
-    <t>Fling Match Lighter Metal Outdoor Camping</t>
+    <t>Flint Match Lighter Metal Outdoor Camping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,21 +393,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="54.7109375" customWidth="1"/>
@@ -415,7 +415,7 @@
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -432,7 +432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -449,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -466,7 +466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Iron Man Cushion Cover pillow sale price 599
</commit_message>
<xml_diff>
--- a/Inventory/inventory.tracker.xlsx
+++ b/Inventory/inventory.tracker.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12645"/>
   </bookViews>
@@ -10,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -52,13 +52,19 @@
   </si>
   <si>
     <t>Flint Match Lighter Metal Outdoor Camping</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>Iron Man Cushion Cover Pillow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,21 +399,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="54.7109375" customWidth="1"/>
@@ -415,7 +421,7 @@
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -432,7 +438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -449,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -466,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -480,6 +486,23 @@
         <v>149</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>350</v>
+      </c>
+      <c r="D5">
+        <v>599</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Iron Man poster [Retro] saleprice 249
</commit_message>
<xml_diff>
--- a/Inventory/inventory.tracker.xlsx
+++ b/Inventory/inventory.tracker.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Iron Man Cushion Cover Pillow</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>Iron  Man Poster [Retro]</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -506,6 +512,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>140</v>
+      </c>
+      <c r="D6">
+        <v>249</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
LED Bicycle Front Head Light Sale price 799
</commit_message>
<xml_diff>
--- a/Inventory/inventory.tracker.xlsx
+++ b/Inventory/inventory.tracker.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Iron  Man Poster [Retro]</t>
+  </si>
+  <si>
+    <t>0006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED Bicyle Front Head Light </t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -413,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,6 +535,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>450</v>
+      </c>
+      <c r="D7">
+        <v>799</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mini Coffee Thermos Bottle [380]Ml saieprice 1.499
</commit_message>
<xml_diff>
--- a/Inventory/inventory.tracker.xlsx
+++ b/Inventory/inventory.tracker.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t xml:space="preserve">LED Bicyle Front Head Light </t>
+  </si>
+  <si>
+    <t>0007</t>
+  </si>
+  <si>
+    <t>Mini Coffee Thermos Bottle [380]Ml</t>
   </si>
 </sst>
 </file>
@@ -411,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -552,6 +558,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>700</v>
+      </c>
+      <c r="D8">
+        <v>1.4990000000000001</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>